<commit_message>
Edición excel mas primera edición Puente Alto
</commit_message>
<xml_diff>
--- a/BBDD Gran Santiago.xlsx
+++ b/BBDD Gran Santiago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos santiago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D806201A-203D-4A25-A22A-6A0BD132779D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D1DD5D-2D5F-4691-84B1-4969DB8EF7A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="302">
   <si>
     <t>STGO</t>
   </si>
@@ -942,9 +942,6 @@
     <t>La Olla de Puente</t>
   </si>
   <si>
-    <t>Bajos de Mena Organizaciones</t>
-  </si>
-  <si>
     <t>Asamblea Villa Valle del Sol</t>
   </si>
   <si>
@@ -964,9 +961,6 @@
   </si>
   <si>
     <t xml:space="preserve">ASAMBLEA TERRITORIAL TRINIDAD </t>
-  </si>
-  <si>
-    <t>Asamblea Mujeres Cordillera</t>
   </si>
   <si>
     <t>Asamblea Protectora</t>
@@ -1063,6 +1057,9 @@
   </si>
   <si>
     <t>Asamblea autoconvocada población Santa Julia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bajos de Mena Organizado </t>
   </si>
 </sst>
 </file>
@@ -60197,10 +60194,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AC1009"/>
+  <dimension ref="A1:AC1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -60377,7 +60374,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="71" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
@@ -60391,7 +60388,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="69" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
@@ -60405,7 +60402,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="69" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
@@ -60419,7 +60416,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="69" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
@@ -60433,7 +60430,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="71" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
@@ -60503,7 +60500,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1">
@@ -60800,7 +60797,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
@@ -60814,7 +60811,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="69" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
@@ -60899,7 +60896,7 @@
         <v>6</v>
       </c>
       <c r="D41" s="69" t="s">
-        <v>262</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
@@ -60913,7 +60910,7 @@
         <v>7</v>
       </c>
       <c r="D42" s="69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
@@ -60927,7 +60924,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1">
@@ -60941,7 +60938,7 @@
         <v>9</v>
       </c>
       <c r="D44" s="69" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1">
@@ -60955,7 +60952,7 @@
         <v>10</v>
       </c>
       <c r="D45" s="69" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
@@ -60969,7 +60966,7 @@
         <v>11</v>
       </c>
       <c r="D46" s="69" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1">
@@ -60983,7 +60980,7 @@
         <v>12</v>
       </c>
       <c r="D47" s="69" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1">
@@ -60997,7 +60994,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="69" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
@@ -61011,7 +61008,7 @@
         <v>14</v>
       </c>
       <c r="D49" s="69" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
@@ -61025,21 +61022,21 @@
         <v>15</v>
       </c>
       <c r="D50" s="69" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="72">
         <v>48</v>
       </c>
-      <c r="B51" s="72" t="s">
-        <v>257</v>
+      <c r="B51" s="71" t="s">
+        <v>270</v>
       </c>
       <c r="C51" s="74">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D51" s="69" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
@@ -61047,24 +61044,24 @@
         <v>49</v>
       </c>
       <c r="B52" s="71" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C52" s="74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="69" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
       <c r="A53" s="72">
         <v>50</v>
       </c>
-      <c r="B53" s="71" t="s">
-        <v>272</v>
+      <c r="B53" s="72" t="s">
+        <v>273</v>
       </c>
       <c r="C53" s="74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" s="69" t="s">
         <v>274</v>
@@ -61075,13 +61072,13 @@
         <v>51</v>
       </c>
       <c r="B54" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C54" s="74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="69" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
@@ -61089,13 +61086,13 @@
         <v>52</v>
       </c>
       <c r="B55" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C55" s="74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D55" s="69" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
@@ -61103,13 +61100,13 @@
         <v>53</v>
       </c>
       <c r="B56" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C56" s="74">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D56" s="69" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
@@ -61117,13 +61114,13 @@
         <v>54</v>
       </c>
       <c r="B57" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C57" s="74">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D57" s="69" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
@@ -61131,13 +61128,13 @@
         <v>55</v>
       </c>
       <c r="B58" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C58" s="74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" s="69" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
@@ -61145,13 +61142,13 @@
         <v>56</v>
       </c>
       <c r="B59" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C59" s="74">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D59" s="69" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
@@ -61159,13 +61156,13 @@
         <v>57</v>
       </c>
       <c r="B60" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C60" s="74">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c r="D60" s="69" t="s">
-        <v>282</v>
+      <c r="D60" s="71" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1">
@@ -61173,13 +61170,13 @@
         <v>58</v>
       </c>
       <c r="B61" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C61" s="74">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="D61" s="71" t="s">
-        <v>283</v>
+      <c r="D61" s="69" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1">
@@ -61187,13 +61184,13 @@
         <v>59</v>
       </c>
       <c r="B62" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C62" s="74">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D62" s="69" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1">
@@ -61201,13 +61198,13 @@
         <v>60</v>
       </c>
       <c r="B63" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C63" s="74">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D63" s="69" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1">
@@ -61215,13 +61212,13 @@
         <v>61</v>
       </c>
       <c r="B64" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C64" s="74">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D64" s="69" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1">
@@ -61229,13 +61226,13 @@
         <v>62</v>
       </c>
       <c r="B65" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C65" s="74">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D65" s="69" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1">
@@ -61243,13 +61240,13 @@
         <v>63</v>
       </c>
       <c r="B66" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C66" s="74">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D66" s="69" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1">
@@ -61257,13 +61254,13 @@
         <v>64</v>
       </c>
       <c r="B67" s="72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C67" s="74">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D67" s="69" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
@@ -61271,10 +61268,10 @@
         <v>65</v>
       </c>
       <c r="B68" s="72" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
-      <c r="C68" s="74">
-        <v>15</v>
+      <c r="C68" s="72">
+        <v>1</v>
       </c>
       <c r="D68" s="69" t="s">
         <v>290</v>
@@ -61285,29 +61282,16 @@
         <v>66</v>
       </c>
       <c r="B69" s="72" t="s">
+        <v>289</v>
+      </c>
+      <c r="C69" s="72">
+        <v>2</v>
+      </c>
+      <c r="D69" s="69" t="s">
         <v>291</v>
       </c>
-      <c r="C69" s="72">
-        <v>1</v>
-      </c>
-      <c r="D69" s="69" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A70" s="72">
-        <v>67</v>
-      </c>
-      <c r="B70" s="72" t="s">
-        <v>291</v>
-      </c>
-      <c r="C70" s="72">
-        <v>2</v>
-      </c>
-      <c r="D70" s="69" t="s">
-        <v>293</v>
-      </c>
-    </row>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="71" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="72" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="73" spans="1:4" ht="15.75" customHeight="1"/>
@@ -62246,7 +62230,6 @@
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
     <row r="1008" ht="15.75" customHeight="1"/>
-    <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:S1"/>

</xml_diff>

<commit_message>
Edición excel y primera edición San Bernardo
</commit_message>
<xml_diff>
--- a/BBDD Gran Santiago.xlsx
+++ b/BBDD Gran Santiago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos santiago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D1DD5D-2D5F-4691-84B1-4969DB8EF7A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734ECD7B-82A4-421C-9E95-43DDD11649C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="301">
   <si>
     <t>STGO</t>
   </si>
@@ -1009,9 +1009,6 @@
   </si>
   <si>
     <t>komiaelmew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asamb Territorial No+AFP Sn Bdo </t>
   </si>
   <si>
     <t>Vecinos en accion San Bernardo</t>
@@ -60194,10 +60191,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AC1008"/>
+  <dimension ref="A1:AC1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -60374,7 +60371,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
@@ -60388,7 +60385,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="69" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
@@ -60402,7 +60399,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
@@ -60416,7 +60413,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
@@ -60430,7 +60427,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
@@ -60500,7 +60497,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1">
@@ -60797,7 +60794,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
@@ -60811,7 +60808,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="69" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
@@ -60896,7 +60893,7 @@
         <v>6</v>
       </c>
       <c r="D41" s="69" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
@@ -61022,7 +61019,7 @@
         <v>15</v>
       </c>
       <c r="D50" s="69" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
@@ -61215,7 +61212,7 @@
         <v>273</v>
       </c>
       <c r="C64" s="74">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D64" s="69" t="s">
         <v>285</v>
@@ -61229,7 +61226,7 @@
         <v>273</v>
       </c>
       <c r="C65" s="74">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D65" s="69" t="s">
         <v>286</v>
@@ -61243,7 +61240,7 @@
         <v>273</v>
       </c>
       <c r="C66" s="74">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D66" s="69" t="s">
         <v>287</v>
@@ -61254,13 +61251,13 @@
         <v>64</v>
       </c>
       <c r="B67" s="72" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
-      <c r="C67" s="74">
-        <v>15</v>
+      <c r="C67" s="72">
+        <v>1</v>
       </c>
       <c r="D67" s="69" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
@@ -61268,29 +61265,16 @@
         <v>65</v>
       </c>
       <c r="B68" s="72" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C68" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D68" s="69" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A69" s="72">
-        <v>66</v>
-      </c>
-      <c r="B69" s="72" t="s">
-        <v>289</v>
-      </c>
-      <c r="C69" s="72">
-        <v>2</v>
-      </c>
-      <c r="D69" s="69" t="s">
-        <v>291</v>
-      </c>
-    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="70" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="71" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="72" spans="1:4" ht="15.75" customHeight="1"/>
@@ -62229,7 +62213,6 @@
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:S1"/>

</xml_diff>

<commit_message>
edición asamblea Elisa Correa
</commit_message>
<xml_diff>
--- a/BBDD Gran Santiago.xlsx
+++ b/BBDD Gran Santiago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos santiago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734ECD7B-82A4-421C-9E95-43DDD11649C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8333161E-DB1D-4107-BC2D-378FF35D8C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1419,7 +1419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1591,6 +1591,7 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -29288,25 +29289,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -29331,11 +29332,11 @@
       <c r="D2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="80"/>
       <c r="H2" s="12" t="s">
         <v>34</v>
       </c>
@@ -58619,25 +58620,25 @@
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1">
       <c r="A1" s="25"/>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="80"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="26" t="s">
@@ -58655,11 +58656,11 @@
       <c r="E2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
       <c r="I2" s="29" t="s">
         <v>34</v>
       </c>
@@ -58766,7 +58767,7 @@
       <c r="AB3" s="35"/>
     </row>
     <row r="4" spans="1:28" ht="182.25" customHeight="1">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="83" t="s">
         <v>135</v>
       </c>
       <c r="B4" s="36" t="s">
@@ -58822,14 +58823,14 @@
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="83" t="s">
+      <c r="A5" s="77"/>
+      <c r="B5" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="85" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="42" t="s">
@@ -58837,25 +58838,25 @@
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A6" s="76"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
       <c r="E6" s="43" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A7" s="76"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
       <c r="E7" s="44" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A8" s="76"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="45" t="s">
         <v>158</v>
       </c>
@@ -60193,8 +60194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -60214,25 +60215,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1">
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="81" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="80"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="68" t="s">
@@ -60253,11 +60254,11 @@
       <c r="F2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="80"/>
       <c r="J2" s="29" t="s">
         <v>34</v>
       </c>
@@ -60404,7 +60405,7 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="72">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="72" t="s">
         <v>228</v>
@@ -60412,619 +60413,619 @@
       <c r="C7" s="72">
         <v>4</v>
       </c>
-      <c r="D7" s="69" t="s">
-        <v>294</v>
+      <c r="D7" s="71" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="72">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="72" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C8" s="72">
-        <v>5</v>
+        <v>1</v>
       </c>
-      <c r="D8" s="71" t="s">
-        <v>295</v>
+      <c r="D8" s="69" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="72">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="72" t="s">
         <v>229</v>
       </c>
       <c r="C9" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1">
       <c r="A10" s="72">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="72" t="s">
         <v>229</v>
       </c>
       <c r="C10" s="72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1">
       <c r="A11" s="72">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="72" t="s">
         <v>229</v>
       </c>
       <c r="C11" s="72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1">
       <c r="A12" s="72">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="72" t="s">
         <v>229</v>
       </c>
       <c r="C12" s="72">
-        <v>4</v>
+        <v>5</v>
       </c>
-      <c r="D12" s="69" t="s">
-        <v>233</v>
+      <c r="D12" s="70" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1">
       <c r="A13" s="72">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="72" t="s">
         <v>229</v>
       </c>
       <c r="C13" s="72">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="D13" s="70" t="s">
-        <v>299</v>
+      <c r="D13" s="69" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1">
       <c r="A14" s="72">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="72" t="s">
         <v>229</v>
       </c>
       <c r="C14" s="72">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="69" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1">
       <c r="A15" s="72">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="72" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
-      <c r="C15" s="72">
-        <v>7</v>
+      <c r="C15" s="73">
+        <v>1</v>
       </c>
-      <c r="D15" s="69" t="s">
-        <v>235</v>
+      <c r="D15" s="71" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1">
       <c r="A16" s="72">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="72" t="s">
         <v>236</v>
       </c>
       <c r="C16" s="73">
-        <v>1</v>
+        <v>2</v>
       </c>
-      <c r="D16" s="71" t="s">
-        <v>237</v>
+      <c r="D16" s="69" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="72">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="72" t="s">
         <v>236</v>
       </c>
       <c r="C17" s="73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="69" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="72">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="72" t="s">
         <v>236</v>
       </c>
       <c r="C18" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" s="69" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="72">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="72" t="s">
         <v>236</v>
       </c>
       <c r="C19" s="73">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="72">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="72" t="s">
         <v>236</v>
       </c>
       <c r="C20" s="73">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="72">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="72" t="s">
         <v>236</v>
       </c>
       <c r="C21" s="73">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21" s="69" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="72">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="72" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C22" s="73">
-        <v>7</v>
+        <v>1</v>
       </c>
-      <c r="D22" s="69" t="s">
-        <v>243</v>
+      <c r="D22" s="71" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="72">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C23" s="73">
-        <v>1</v>
+        <v>2</v>
       </c>
-      <c r="D23" s="71" t="s">
-        <v>244</v>
+      <c r="D23" s="69" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="72">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C24" s="73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="69" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
+      <c r="F24" s="48"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="72">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C25" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="69" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
-      <c r="F25" s="48"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="72">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C26" s="73">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" s="69" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
-      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="72">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C27" s="73">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27" s="69" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="72">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C28" s="73">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" s="69" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="72">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C29" s="73">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" s="69" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="72">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C30" s="73">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D30" s="69" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
-      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="72">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C31" s="73">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" s="69" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="72">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C32" s="73">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D32" s="69" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="72">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C33" s="73">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33" s="69" t="s">
-        <v>255</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="72">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="72" t="s">
         <v>245</v>
       </c>
       <c r="C34" s="73">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="72">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="72" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
-      <c r="C35" s="73">
-        <v>13</v>
+      <c r="C35" s="74">
+        <v>1</v>
       </c>
-      <c r="D35" s="69" t="s">
-        <v>298</v>
+      <c r="D35" s="71" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="72">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C36" s="74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D36" s="71" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="72">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C37" s="74">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="D37" s="71" t="s">
-        <v>258</v>
+      <c r="D37" s="69" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="72">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C38" s="74">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38" s="69" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="72">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C39" s="74">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D39" s="69" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
-      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="72">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C40" s="74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D40" s="69" t="s">
-        <v>261</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="72">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C41" s="74">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D41" s="69" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="72">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C42" s="74">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42" s="69" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="72">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C43" s="74">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D43" s="69" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="72">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C44" s="74">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D44" s="69" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="72">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C45" s="74">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D45" s="69" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="72">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C46" s="74">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46" s="69" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="72">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C47" s="74">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D47" s="69" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="72">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C48" s="74">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D48" s="69" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="72">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C49" s="74">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D49" s="69" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+    <row r="50" spans="1:4" s="75" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="72">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50" s="72" t="s">
         <v>257</v>
       </c>
       <c r="C50" s="74">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D50" s="69" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="72">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51" s="71" t="s">
         <v>270</v>
@@ -61038,7 +61039,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
       <c r="A52" s="72">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B52" s="71" t="s">
         <v>270</v>
@@ -61052,7 +61053,7 @@
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
       <c r="A53" s="72">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" s="72" t="s">
         <v>273</v>
@@ -61066,7 +61067,7 @@
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
       <c r="A54" s="72">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" s="72" t="s">
         <v>273</v>
@@ -61080,7 +61081,7 @@
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
       <c r="A55" s="72">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B55" s="72" t="s">
         <v>273</v>
@@ -61094,7 +61095,7 @@
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
       <c r="A56" s="72">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B56" s="72" t="s">
         <v>273</v>
@@ -61108,7 +61109,7 @@
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
       <c r="A57" s="72">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57" s="72" t="s">
         <v>273</v>
@@ -61122,7 +61123,7 @@
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
       <c r="A58" s="72">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B58" s="72" t="s">
         <v>273</v>
@@ -61136,7 +61137,7 @@
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
       <c r="A59" s="72">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B59" s="72" t="s">
         <v>273</v>
@@ -61150,7 +61151,7 @@
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
       <c r="A60" s="72">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60" s="72" t="s">
         <v>273</v>
@@ -61164,7 +61165,7 @@
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1">
       <c r="A61" s="72">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B61" s="72" t="s">
         <v>273</v>
@@ -61178,7 +61179,7 @@
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1">
       <c r="A62" s="72">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B62" s="72" t="s">
         <v>273</v>
@@ -61192,7 +61193,7 @@
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1">
       <c r="A63" s="72">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B63" s="72" t="s">
         <v>273</v>
@@ -61206,7 +61207,7 @@
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1">
       <c r="A64" s="72">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B64" s="72" t="s">
         <v>273</v>
@@ -61220,7 +61221,7 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1">
       <c r="A65" s="72">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B65" s="72" t="s">
         <v>273</v>
@@ -61234,7 +61235,7 @@
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1">
       <c r="A66" s="72">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B66" s="72" t="s">
         <v>273</v>
@@ -61248,7 +61249,7 @@
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1">
       <c r="A67" s="72">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B67" s="72" t="s">
         <v>288</v>
@@ -61262,7 +61263,7 @@
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
       <c r="A68" s="72">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B68" s="72" t="s">
         <v>288</v>

</xml_diff>